<commit_message>
Corrects mistakes (and changes of mind)
</commit_message>
<xml_diff>
--- a/dat/variable_correspondence.xlsx
+++ b/dat/variable_correspondence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>setting</t>
   </si>
@@ -188,7 +188,25 @@
     <t>Interesting for researchers but not available anywhere</t>
   </si>
   <si>
-    <t>Could be of interest although maybe not one of the most important ones, but I would NOT include it because we could save integrating the file sent by Ellen</t>
+    <t>socioEnvContextOther</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Complement socioEnvContext</t>
+  </si>
+  <si>
+    <t>methodology.analysesOther</t>
+  </si>
+  <si>
+    <t>AQ</t>
+  </si>
+  <si>
+    <t>Complement methodology.analyses</t>
+  </si>
+  <si>
+    <t>Could be of interest although maybe not one of the most important ones</t>
   </si>
 </sst>
 </file>
@@ -232,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -241,6 +259,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,21 +540,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="52.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="142" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="127.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="146.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -612,109 +631,109 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
       <c r="L7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="L9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
       </c>
       <c r="F10" t="s">
         <v>27</v>
       </c>
       <c r="L10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
         <v>27</v>
@@ -722,16 +741,10 @@
       <c r="L11" t="s">
         <v>33</v>
       </c>
-      <c r="M11" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
         <v>27</v>
@@ -741,34 +754,28 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="L13" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="M13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
@@ -777,39 +784,79 @@
         <v>27</v>
       </c>
       <c r="L14" t="s">
-        <v>54</v>
-      </c>
-      <c r="M14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L17" t="s">
         <v>53</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M17" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="F1:K1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Includes column with Angel's suggestions about variables to include
</commit_message>
<xml_diff>
--- a/dat/variable_correspondence.xlsx
+++ b/dat/variable_correspondence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>setting</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>Could be of interest although maybe not one of the most important ones</t>
+  </si>
+  <si>
+    <t>Ángel</t>
+  </si>
+  <si>
+    <t>YES/NO</t>
   </si>
 </sst>
 </file>
@@ -253,13 +259,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +549,10 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,47 +568,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="3" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="2"/>
+      <c r="G2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -614,6 +626,9 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
       <c r="L3" t="s">
         <v>21</v>
       </c>
@@ -631,7 +646,10 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -662,6 +680,9 @@
       <c r="F6" t="s">
         <v>13</v>
       </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
       <c r="L6" t="s">
         <v>24</v>
       </c>
@@ -693,6 +714,9 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
       <c r="L8" t="s">
         <v>26</v>
       </c>
@@ -710,6 +734,9 @@
       <c r="F9" t="s">
         <v>13</v>
       </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
       <c r="L9" t="s">
         <v>26</v>
       </c>
@@ -724,6 +751,9 @@
       <c r="F10" t="s">
         <v>27</v>
       </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
       <c r="L10" t="s">
         <v>28</v>
       </c>
@@ -738,6 +768,9 @@
       <c r="F11" t="s">
         <v>27</v>
       </c>
+      <c r="G11" t="s">
+        <v>62</v>
+      </c>
       <c r="L11" t="s">
         <v>33</v>
       </c>
@@ -749,6 +782,9 @@
       <c r="F12" t="s">
         <v>27</v>
       </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
       <c r="L12" t="s">
         <v>31</v>
       </c>
@@ -766,6 +802,9 @@
       <c r="F13" t="s">
         <v>27</v>
       </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
       <c r="L13" t="s">
         <v>33</v>
       </c>
@@ -783,6 +822,9 @@
       <c r="F14" t="s">
         <v>27</v>
       </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
       <c r="L14" t="s">
         <v>31</v>
       </c>
@@ -806,6 +848,9 @@
       <c r="F15" t="s">
         <v>13</v>
       </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
       <c r="L15" t="s">
         <v>26</v>
       </c>
@@ -823,6 +868,9 @@
       <c r="F16" t="s">
         <v>13</v>
       </c>
+      <c r="G16" t="s">
+        <v>62</v>
+      </c>
       <c r="L16" t="s">
         <v>60</v>
       </c>
@@ -837,8 +885,11 @@
       <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
       </c>
       <c r="L17" t="s">
         <v>53</v>

</xml_diff>